<commit_message>
merapihkn template permohonan dinas dan puskesmas
</commit_message>
<xml_diff>
--- a/dinas/public/files/template/inventory/permohonan_barang.xlsx
+++ b/dinas/public/files/template/inventory/permohonan_barang.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\projek\epuskesmasgarut\public\files\template\inventory\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\projek\inovasi\garut\dinas\public\files\template\inventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -81,7 +81,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,6 +97,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF444444"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color rgb="FF444444"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -135,12 +142,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -163,8 +173,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B6:H7" totalsRowShown="0">
-  <autoFilter ref="B6:H7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A6:G7" totalsRowShown="0">
+  <autoFilter ref="A6:G7"/>
   <tableColumns count="7">
     <tableColumn id="1" name="No"/>
     <tableColumn id="2" name="Tanggal Permohonan" dataDxfId="0"/>
@@ -254,6 +264,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -289,6 +316,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -441,87 +485,97 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H7"/>
+  <dimension ref="A2:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="6.140625" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
-    <col min="5" max="6" width="16.28515625" customWidth="1"/>
-    <col min="7" max="7" width="36" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" customWidth="1"/>
+    <col min="6" max="6" width="28.28515625" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>14</v>
       </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="2:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
+    <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
       <c r="B6" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="G6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F7" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:G2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="70" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>